<commit_message>
Started changing according to fields to use in SVV
</commit_message>
<xml_diff>
--- a/working-files-data/package_create.xlsx
+++ b/working-files-data/package_create.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HILAUS\GitHub\svv-ckan-setup\synced_folders\src\test\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HILAUS\GitHub\svv-ckan-setup\synced_folders\src\svv-ckan-import\working-files-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="226">
   <si>
     <t>title</t>
   </si>
@@ -463,12 +463,6 @@
     <t>author_email</t>
   </si>
   <si>
-    <t>Bruker ikke denne</t>
-  </si>
-  <si>
-    <t>nope@invalid.com</t>
-  </si>
-  <si>
     <t>subject</t>
   </si>
   <si>
@@ -479,9 +473,6 @@
   </si>
   <si>
     <t>alternate_identifier</t>
-  </si>
-  <si>
-    <t>Tja</t>
   </si>
   <si>
     <t>issued</t>
@@ -502,24 +493,6 @@
     <t>creator</t>
   </si>
   <si>
-    <t>2016-01-01</t>
-  </si>
-  <si>
-    <t>2000-01-01</t>
-  </si>
-  <si>
-    <t>2010-12-31</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>Denne er bedre enn den forrige</t>
-  </si>
-  <si>
-    <t>Tja, noen andre?</t>
-  </si>
-  <si>
     <t>provenance</t>
   </si>
   <si>
@@ -532,13 +505,7 @@
     <t>modified</t>
   </si>
   <si>
-    <t>2016-10-01</t>
-  </si>
-  <si>
     <t>ANNUAL</t>
-  </si>
-  <si>
-    <t>Samlet opp langs vegkanten</t>
   </si>
   <si>
     <t>http://vegdata.no</t>
@@ -698,6 +665,39 @@
   </si>
   <si>
     <t>http://publications.europa.eu/resource/authority/access-right/PUBLIC</t>
+  </si>
+  <si>
+    <t>obligatorisk i dcat</t>
+  </si>
+  <si>
+    <t>obligatorisk i ckan</t>
+  </si>
+  <si>
+    <t>anbefalt i svv</t>
+  </si>
+  <si>
+    <t>obligatorisk i svv - bruke org-enhet</t>
+  </si>
+  <si>
+    <t>obligatorisk i svv</t>
+  </si>
+  <si>
+    <t>hm</t>
+  </si>
+  <si>
+    <t>obligatorisk i svv - bruke felles-epost?</t>
+  </si>
+  <si>
+    <t>krever</t>
+  </si>
+  <si>
+    <t>er påkrevd av</t>
+  </si>
+  <si>
+    <t>erstatter</t>
+  </si>
+  <si>
+    <t>erstattes av</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1202,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1223,6 +1223,9 @@
     <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1269,7 +1272,30 @@
     <cellStyle name="Uthevingsfarge6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Varseltekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1545,13 +1571,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH34"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J25" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14 A1:XFD1"/>
-      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
+      <selection pane="bottomRight" activeCell="V1" sqref="V1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1560,1566 +1586,1583 @@
     <col min="2" max="2" width="31.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="56" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
-    <col min="6" max="9" width="11" style="1"/>
+    <col min="5" max="9" width="12.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="22.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="42.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="53.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.25" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11" style="1"/>
+    <col min="11" max="11" width="15.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="42.125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="53.75" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.25" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:25" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G2" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="S1" s="7" t="s">
-        <v>144</v>
+      <c r="T2" s="6" t="s">
+        <v>148</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="V1" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="W1" s="6" t="s">
-        <v>150</v>
+      <c r="V2" s="6" t="s">
+        <v>222</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>151</v>
+      <c r="W2" s="6" t="s">
+        <v>223</v>
       </c>
-      <c r="Y1" s="6" t="s">
-        <v>152</v>
+      <c r="X2" s="6" t="s">
+        <v>224</v>
       </c>
-      <c r="Z1" s="6" t="s">
-        <v>154</v>
+      <c r="Y2" s="6" t="s">
+        <v>225</v>
       </c>
-      <c r="AA1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" t="s">
-        <v>177</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>127</v>
+      <c r="G3" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L3" t="s">
-        <v>176</v>
+      <c r="K3" s="1" t="s">
+        <v>84</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>224</v>
+      <c r="M3" t="s">
+        <v>166</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>220</v>
+      <c r="R3" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S3" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:25" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>47</v>
+      <c r="G4" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>178</v>
+      <c r="K4" s="1" t="s">
+        <v>47</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>224</v>
+      <c r="M4" t="s">
+        <v>165</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q4" s="4" t="s">
-        <v>220</v>
+      <c r="R4" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S4" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:25" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>126</v>
+      <c r="M5" s="5" t="s">
+        <v>167</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>127</v>
+      <c r="O5" s="5" t="s">
+        <v>213</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="L5" t="s">
-        <v>174</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
-      <c r="S5" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>225</v>
+      <c r="M6" t="s">
+        <v>163</v>
       </c>
-      <c r="L6" t="s">
-        <v>179</v>
+      <c r="N6" s="4" t="s">
+        <v>162</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>224</v>
+      <c r="O6" s="5" t="s">
+        <v>213</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q6" s="4" t="s">
-        <v>220</v>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4" t="s">
+        <v>210</v>
       </c>
-      <c r="S6" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>225</v>
+      <c r="M7" t="s">
+        <v>168</v>
       </c>
-      <c r="L7" t="s">
-        <v>180</v>
+      <c r="O7" s="5" t="s">
+        <v>213</v>
       </c>
-      <c r="N7" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q7" s="4" t="s">
-        <v>220</v>
+      <c r="R7" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S7" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
+      <c r="G8" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="L8" t="s">
-        <v>181</v>
+      <c r="K8" s="1" t="s">
+        <v>47</v>
       </c>
-      <c r="N8" s="5" t="s">
-        <v>224</v>
+      <c r="M8" t="s">
+        <v>169</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q8" s="4" t="s">
-        <v>220</v>
+      <c r="R8" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S8" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>103</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>95</v>
+      <c r="G9" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>182</v>
+      <c r="K9" s="1" t="s">
+        <v>33</v>
       </c>
-      <c r="N9" s="5" t="s">
-        <v>224</v>
+      <c r="M9" t="s">
+        <v>170</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q9" s="4" t="s">
-        <v>220</v>
+      <c r="R9" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S9" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>122</v>
+      <c r="G10" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="L10" t="s">
-        <v>183</v>
+      <c r="K10" s="1" t="s">
+        <v>95</v>
       </c>
-      <c r="N10" s="5" t="s">
-        <v>224</v>
+      <c r="M10" s="5" t="s">
+        <v>171</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q10" s="4" t="s">
-        <v>220</v>
+      <c r="R10" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S10" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:25" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>47</v>
+      <c r="G11" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="L11" t="s">
-        <v>184</v>
+      <c r="K11" s="1" t="s">
+        <v>124</v>
       </c>
-      <c r="N11" s="5" t="s">
-        <v>224</v>
+      <c r="M11" t="s">
+        <v>172</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q11" s="4" t="s">
-        <v>220</v>
+      <c r="R11" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S11" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>84</v>
+      <c r="G12" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="L12" t="s">
-        <v>185</v>
+      <c r="K12" s="1" t="s">
+        <v>47</v>
       </c>
-      <c r="N12" s="5" t="s">
-        <v>224</v>
+      <c r="M12" t="s">
+        <v>173</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q12" s="4" t="s">
-        <v>220</v>
+      <c r="R12" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S12" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:25" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>47</v>
+      <c r="G13" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>175</v>
+      <c r="K13" s="1" t="s">
+        <v>84</v>
       </c>
-      <c r="N13" s="5" t="s">
-        <v>224</v>
+      <c r="M13" t="s">
+        <v>174</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q13" s="4" t="s">
-        <v>220</v>
+      <c r="R13" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="S13" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>33</v>
+      <c r="G14" s="4" t="s">
+        <v>187</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>130</v>
+      <c r="K14" s="1" t="s">
+        <v>47</v>
       </c>
-      <c r="N14" s="5" t="s">
-        <v>224</v>
+      <c r="M14" s="5" t="s">
+        <v>164</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="O14" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="S14" s="4" t="s">
-        <v>200</v>
+      <c r="R14" s="4" t="s">
+        <v>209</v>
       </c>
-      <c r="W14" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>93</v>
+      <c r="G15" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N15" s="5" t="s">
-        <v>224</v>
+      <c r="K15" s="1" t="s">
+        <v>33</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="M15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>121</v>
+      <c r="Q15" s="1" t="s">
+        <v>120</v>
       </c>
-      <c r="S15" s="4" t="s">
-        <v>201</v>
+      <c r="T15" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
+      <c r="G16" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N16" s="5" t="s">
-        <v>224</v>
+      <c r="K16" s="1" t="s">
+        <v>93</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="O16" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S16" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" ht="63.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>225</v>
+      <c r="O17" s="5" t="s">
+        <v>213</v>
       </c>
-      <c r="N17" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S17" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:17" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>33</v>
+      <c r="G18" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N18" s="5" t="s">
-        <v>224</v>
+      <c r="K18" s="1" t="s">
+        <v>47</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S18" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>128</v>
+      <c r="G19" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N19" s="5" t="s">
-        <v>224</v>
+      <c r="K19" s="1" t="s">
+        <v>33</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="O19" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P19" s="1" t="s">
-        <v>120</v>
+      <c r="Q19" s="1" t="s">
+        <v>121</v>
       </c>
-      <c r="S19" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="2:17" ht="51" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>47</v>
+      <c r="G20" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N20" s="5" t="s">
-        <v>224</v>
+      <c r="K20" s="1" t="s">
+        <v>39</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>117</v>
+      <c r="O20" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>121</v>
+        <v>20</v>
       </c>
-      <c r="S20" s="4" t="s">
-        <v>206</v>
+      <c r="Q20" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="21" spans="2:19" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>39</v>
+      <c r="G21" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N21" s="5" t="s">
-        <v>224</v>
+      <c r="K21" s="1" t="s">
+        <v>47</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>20</v>
+      <c r="O21" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="P21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S21" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="2:17" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>84</v>
+      <c r="G22" s="4" t="s">
+        <v>196</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N22" s="5" t="s">
-        <v>224</v>
+      <c r="K22" s="1" t="s">
+        <v>39</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="O22" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S22" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>94</v>
+      <c r="G23" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N23" s="5" t="s">
-        <v>224</v>
+      <c r="K23" s="1" t="s">
+        <v>84</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="O23" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S23" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J24" s="4" t="s">
-        <v>225</v>
+      <c r="O24" s="5" t="s">
+        <v>213</v>
       </c>
-      <c r="N24" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S24" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="25" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>39</v>
+      <c r="G25" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N25" s="5" t="s">
-        <v>224</v>
+      <c r="K25" s="1" t="s">
+        <v>94</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="O25" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S25" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="2:17" ht="51" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>47</v>
+      <c r="G26" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N26" s="5" t="s">
-        <v>224</v>
+      <c r="K26" s="1" t="s">
+        <v>39</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="O26" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S26" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>93</v>
+      <c r="G27" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N27" s="5" t="s">
-        <v>224</v>
+      <c r="K27" s="1" t="s">
+        <v>47</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="O27" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S27" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>84</v>
+      <c r="G28" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N28" s="5" t="s">
-        <v>224</v>
+      <c r="K28" s="1" t="s">
+        <v>93</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="O28" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S28" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>95</v>
+      <c r="G29" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N29" s="5" t="s">
-        <v>224</v>
+      <c r="K29" s="1" t="s">
+        <v>84</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="O29" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S29" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>124</v>
+      <c r="G30" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N30" s="5" t="s">
-        <v>224</v>
+      <c r="K30" s="1" t="s">
+        <v>95</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="O30" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S30" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="2:17" ht="51" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>95</v>
+      <c r="G31" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N31" s="5" t="s">
-        <v>224</v>
+      <c r="K31" s="1" t="s">
+        <v>124</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="O31" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="S31" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>33</v>
+      <c r="G32" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
-      <c r="N32" s="5" t="s">
-        <v>224</v>
+      <c r="K32" s="1" t="s">
+        <v>95</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="O32" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>120</v>
+      <c r="Q32" s="1" t="s">
+        <v>121</v>
       </c>
-      <c r="S32" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="33" spans="2:34" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J33" s="4" t="s">
-        <v>225</v>
+      <c r="O33" s="5" t="s">
+        <v>213</v>
       </c>
-      <c r="N33" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="O33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="2:30" ht="51" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q34" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="S33" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="34" spans="2:34" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="9" t="s">
+    </row>
+    <row r="35" spans="2:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F35" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G35" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="K35" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H34" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="K34" s="9" t="s">
+      <c r="L35" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="L34" s="9" t="s">
+      <c r="M35" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="M34" s="9" t="s">
+      <c r="N35" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="N34" s="5" t="s">
-        <v>224</v>
+      <c r="O35" s="5" t="s">
+        <v>213</v>
       </c>
-      <c r="O34" s="9" t="s">
+      <c r="P35" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P34" s="9" t="s">
+      <c r="Q35" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="Q34" s="11" t="s">
-        <v>222</v>
+      <c r="R35" s="11" t="s">
+        <v>211</v>
       </c>
-      <c r="R34" s="11" t="s">
-        <v>222</v>
+      <c r="S35" s="11" t="s">
+        <v>211</v>
       </c>
-      <c r="S34" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="T34" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="U34" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="V34" s="12" t="s">
+      <c r="T35" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="W34" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="X34" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="Y34" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="Z34" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA34" s="9" t="s">
+      <c r="U35" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="AB34" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="AC34" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="AD34" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="AE34" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="AF34" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="AG34" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="AH34" s="9" t="s">
-        <v>170</v>
-      </c>
+      <c r="AD35" s="12"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AH34">
-    <sortCondition ref="L2:L34"/>
+  <sortState ref="A2:AI34">
+    <sortCondition ref="M2:M34"/>
   </sortState>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="obligatorisk">
+      <formula>NOT(ISERROR(SEARCH("obligatorisk",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="M5" r:id="rId1"/>
-    <hyperlink ref="L13" r:id="rId2"/>
-    <hyperlink ref="L9" r:id="rId3"/>
-    <hyperlink ref="S2" r:id="rId4"/>
-    <hyperlink ref="S3" r:id="rId5"/>
-    <hyperlink ref="S4" r:id="rId6"/>
-    <hyperlink ref="S5" r:id="rId7"/>
-    <hyperlink ref="S6" r:id="rId8"/>
-    <hyperlink ref="S7" r:id="rId9"/>
-    <hyperlink ref="S8" r:id="rId10"/>
-    <hyperlink ref="S9" r:id="rId11"/>
-    <hyperlink ref="S10" r:id="rId12"/>
-    <hyperlink ref="S11" r:id="rId13"/>
-    <hyperlink ref="S12" r:id="rId14"/>
-    <hyperlink ref="S13" r:id="rId15"/>
-    <hyperlink ref="S34" r:id="rId16"/>
-    <hyperlink ref="S14" r:id="rId17"/>
-    <hyperlink ref="S15" r:id="rId18"/>
-    <hyperlink ref="S16" r:id="rId19"/>
-    <hyperlink ref="S17" r:id="rId20"/>
-    <hyperlink ref="S18" r:id="rId21"/>
-    <hyperlink ref="S19" r:id="rId22"/>
-    <hyperlink ref="S20" r:id="rId23"/>
-    <hyperlink ref="S21" r:id="rId24"/>
-    <hyperlink ref="S22" r:id="rId25"/>
-    <hyperlink ref="S23" r:id="rId26"/>
-    <hyperlink ref="S24" r:id="rId27"/>
-    <hyperlink ref="S25" r:id="rId28"/>
-    <hyperlink ref="S26" r:id="rId29"/>
-    <hyperlink ref="S27" r:id="rId30"/>
-    <hyperlink ref="S28" r:id="rId31"/>
-    <hyperlink ref="S29" r:id="rId32"/>
-    <hyperlink ref="S30" r:id="rId33"/>
-    <hyperlink ref="S31" r:id="rId34"/>
-    <hyperlink ref="S32" r:id="rId35"/>
-    <hyperlink ref="S33" r:id="rId36"/>
-    <hyperlink ref="Q2" r:id="rId37"/>
-    <hyperlink ref="Q3" r:id="rId38"/>
-    <hyperlink ref="Q4" r:id="rId39"/>
-    <hyperlink ref="Q6" r:id="rId40"/>
-    <hyperlink ref="R5" r:id="rId41"/>
-    <hyperlink ref="Q7" r:id="rId42"/>
-    <hyperlink ref="Q8" r:id="rId43"/>
-    <hyperlink ref="Q9" r:id="rId44"/>
-    <hyperlink ref="Q10" r:id="rId45"/>
-    <hyperlink ref="Q11" r:id="rId46"/>
-    <hyperlink ref="Q12" r:id="rId47"/>
-    <hyperlink ref="Q13" r:id="rId48"/>
-    <hyperlink ref="Q34" r:id="rId49"/>
-    <hyperlink ref="R34" r:id="rId50"/>
-    <hyperlink ref="F2" r:id="rId51"/>
-    <hyperlink ref="F3" r:id="rId52"/>
-    <hyperlink ref="F4" r:id="rId53"/>
-    <hyperlink ref="F5" r:id="rId54"/>
-    <hyperlink ref="F6" r:id="rId55"/>
-    <hyperlink ref="F7" r:id="rId56"/>
-    <hyperlink ref="F8" r:id="rId57"/>
-    <hyperlink ref="F9" r:id="rId58"/>
-    <hyperlink ref="F10" r:id="rId59"/>
-    <hyperlink ref="F33" r:id="rId60"/>
-    <hyperlink ref="F32" r:id="rId61"/>
-    <hyperlink ref="F31" r:id="rId62"/>
-    <hyperlink ref="F30" r:id="rId63"/>
-    <hyperlink ref="F29" r:id="rId64"/>
-    <hyperlink ref="F28" r:id="rId65"/>
-    <hyperlink ref="F16" r:id="rId66"/>
-    <hyperlink ref="F17" r:id="rId67"/>
-    <hyperlink ref="F18" r:id="rId68"/>
-    <hyperlink ref="F19" r:id="rId69"/>
-    <hyperlink ref="F20" r:id="rId70"/>
-    <hyperlink ref="F21" r:id="rId71"/>
-    <hyperlink ref="F22" r:id="rId72"/>
-    <hyperlink ref="F23" r:id="rId73"/>
-    <hyperlink ref="F24" r:id="rId74"/>
-    <hyperlink ref="F25" r:id="rId75"/>
-    <hyperlink ref="F26" r:id="rId76"/>
-    <hyperlink ref="F27" r:id="rId77"/>
-    <hyperlink ref="F11" r:id="rId78"/>
-    <hyperlink ref="F12" r:id="rId79"/>
-    <hyperlink ref="F13" r:id="rId80"/>
-    <hyperlink ref="F14" r:id="rId81"/>
-    <hyperlink ref="F15" r:id="rId82"/>
-    <hyperlink ref="N2" r:id="rId83"/>
-    <hyperlink ref="N3" r:id="rId84"/>
-    <hyperlink ref="N4" r:id="rId85"/>
-    <hyperlink ref="N5" r:id="rId86"/>
-    <hyperlink ref="N6" r:id="rId87"/>
-    <hyperlink ref="N7" r:id="rId88"/>
-    <hyperlink ref="N8" r:id="rId89"/>
-    <hyperlink ref="N9" r:id="rId90"/>
-    <hyperlink ref="N10" r:id="rId91"/>
-    <hyperlink ref="N11" r:id="rId92"/>
-    <hyperlink ref="N12" r:id="rId93"/>
-    <hyperlink ref="N13" r:id="rId94"/>
-    <hyperlink ref="N34" r:id="rId95"/>
-    <hyperlink ref="N14" r:id="rId96"/>
-    <hyperlink ref="N33" r:id="rId97"/>
-    <hyperlink ref="N32" r:id="rId98"/>
-    <hyperlink ref="N31" r:id="rId99"/>
-    <hyperlink ref="N30" r:id="rId100"/>
-    <hyperlink ref="N29" r:id="rId101"/>
-    <hyperlink ref="N28" r:id="rId102"/>
-    <hyperlink ref="N27" r:id="rId103"/>
-    <hyperlink ref="N26" r:id="rId104"/>
-    <hyperlink ref="N25" r:id="rId105"/>
-    <hyperlink ref="N24" r:id="rId106"/>
-    <hyperlink ref="N23" r:id="rId107"/>
-    <hyperlink ref="N22" r:id="rId108"/>
-    <hyperlink ref="N21" r:id="rId109"/>
-    <hyperlink ref="N20" r:id="rId110"/>
-    <hyperlink ref="N19" r:id="rId111"/>
-    <hyperlink ref="N18" r:id="rId112"/>
-    <hyperlink ref="N17" r:id="rId113"/>
-    <hyperlink ref="N16" r:id="rId114"/>
-    <hyperlink ref="N15" r:id="rId115"/>
-    <hyperlink ref="J5" r:id="rId116"/>
-    <hyperlink ref="J6:J33" r:id="rId117" display="http://publications.europa.eu/resource/authority/access-right/PUBLIC"/>
-    <hyperlink ref="J34" r:id="rId118"/>
+    <hyperlink ref="N6" r:id="rId1"/>
+    <hyperlink ref="M14" r:id="rId2"/>
+    <hyperlink ref="M10" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="G4" r:id="rId5"/>
+    <hyperlink ref="G5" r:id="rId6"/>
+    <hyperlink ref="G6" r:id="rId7"/>
+    <hyperlink ref="G7" r:id="rId8"/>
+    <hyperlink ref="G8" r:id="rId9"/>
+    <hyperlink ref="G9" r:id="rId10"/>
+    <hyperlink ref="G10" r:id="rId11"/>
+    <hyperlink ref="G11" r:id="rId12"/>
+    <hyperlink ref="G12" r:id="rId13"/>
+    <hyperlink ref="G13" r:id="rId14"/>
+    <hyperlink ref="G14" r:id="rId15"/>
+    <hyperlink ref="G35" r:id="rId16"/>
+    <hyperlink ref="G15" r:id="rId17"/>
+    <hyperlink ref="G16" r:id="rId18"/>
+    <hyperlink ref="G17" r:id="rId19"/>
+    <hyperlink ref="G18" r:id="rId20"/>
+    <hyperlink ref="G19" r:id="rId21"/>
+    <hyperlink ref="G20" r:id="rId22"/>
+    <hyperlink ref="G21" r:id="rId23"/>
+    <hyperlink ref="G22" r:id="rId24"/>
+    <hyperlink ref="G23" r:id="rId25"/>
+    <hyperlink ref="G24" r:id="rId26"/>
+    <hyperlink ref="G25" r:id="rId27"/>
+    <hyperlink ref="G26" r:id="rId28"/>
+    <hyperlink ref="G27" r:id="rId29"/>
+    <hyperlink ref="G28" r:id="rId30"/>
+    <hyperlink ref="G29" r:id="rId31"/>
+    <hyperlink ref="G30" r:id="rId32"/>
+    <hyperlink ref="G31" r:id="rId33"/>
+    <hyperlink ref="G32" r:id="rId34"/>
+    <hyperlink ref="G33" r:id="rId35"/>
+    <hyperlink ref="G34" r:id="rId36"/>
+    <hyperlink ref="R3" r:id="rId37"/>
+    <hyperlink ref="R4" r:id="rId38"/>
+    <hyperlink ref="R5" r:id="rId39"/>
+    <hyperlink ref="R7" r:id="rId40"/>
+    <hyperlink ref="S6" r:id="rId41"/>
+    <hyperlink ref="R8" r:id="rId42"/>
+    <hyperlink ref="R9" r:id="rId43"/>
+    <hyperlink ref="R10" r:id="rId44"/>
+    <hyperlink ref="R11" r:id="rId45"/>
+    <hyperlink ref="R12" r:id="rId46"/>
+    <hyperlink ref="R13" r:id="rId47"/>
+    <hyperlink ref="R14" r:id="rId48"/>
+    <hyperlink ref="R35" r:id="rId49"/>
+    <hyperlink ref="S35" r:id="rId50"/>
+    <hyperlink ref="F3" r:id="rId51"/>
+    <hyperlink ref="F4" r:id="rId52"/>
+    <hyperlink ref="F5" r:id="rId53"/>
+    <hyperlink ref="F6" r:id="rId54"/>
+    <hyperlink ref="F7" r:id="rId55"/>
+    <hyperlink ref="F8" r:id="rId56"/>
+    <hyperlink ref="F9" r:id="rId57"/>
+    <hyperlink ref="F10" r:id="rId58"/>
+    <hyperlink ref="F11" r:id="rId59"/>
+    <hyperlink ref="F34" r:id="rId60"/>
+    <hyperlink ref="F33" r:id="rId61"/>
+    <hyperlink ref="F32" r:id="rId62"/>
+    <hyperlink ref="F31" r:id="rId63"/>
+    <hyperlink ref="F30" r:id="rId64"/>
+    <hyperlink ref="F29" r:id="rId65"/>
+    <hyperlink ref="F17" r:id="rId66"/>
+    <hyperlink ref="F18" r:id="rId67"/>
+    <hyperlink ref="F19" r:id="rId68"/>
+    <hyperlink ref="F20" r:id="rId69"/>
+    <hyperlink ref="F21" r:id="rId70"/>
+    <hyperlink ref="F22" r:id="rId71"/>
+    <hyperlink ref="F23" r:id="rId72"/>
+    <hyperlink ref="F24" r:id="rId73"/>
+    <hyperlink ref="F25" r:id="rId74"/>
+    <hyperlink ref="F26" r:id="rId75"/>
+    <hyperlink ref="F27" r:id="rId76"/>
+    <hyperlink ref="F28" r:id="rId77"/>
+    <hyperlink ref="F12" r:id="rId78"/>
+    <hyperlink ref="F13" r:id="rId79"/>
+    <hyperlink ref="F14" r:id="rId80"/>
+    <hyperlink ref="F15" r:id="rId81"/>
+    <hyperlink ref="F16" r:id="rId82"/>
+    <hyperlink ref="O3" r:id="rId83"/>
+    <hyperlink ref="O4" r:id="rId84"/>
+    <hyperlink ref="O5" r:id="rId85"/>
+    <hyperlink ref="O6" r:id="rId86"/>
+    <hyperlink ref="O7" r:id="rId87"/>
+    <hyperlink ref="O8" r:id="rId88"/>
+    <hyperlink ref="O9" r:id="rId89"/>
+    <hyperlink ref="O10" r:id="rId90"/>
+    <hyperlink ref="O11" r:id="rId91"/>
+    <hyperlink ref="O12" r:id="rId92"/>
+    <hyperlink ref="O13" r:id="rId93"/>
+    <hyperlink ref="O14" r:id="rId94"/>
+    <hyperlink ref="O35" r:id="rId95"/>
+    <hyperlink ref="O15" r:id="rId96"/>
+    <hyperlink ref="O34" r:id="rId97"/>
+    <hyperlink ref="O33" r:id="rId98"/>
+    <hyperlink ref="O32" r:id="rId99"/>
+    <hyperlink ref="O31" r:id="rId100"/>
+    <hyperlink ref="O30" r:id="rId101"/>
+    <hyperlink ref="O29" r:id="rId102"/>
+    <hyperlink ref="O28" r:id="rId103"/>
+    <hyperlink ref="O27" r:id="rId104"/>
+    <hyperlink ref="O26" r:id="rId105"/>
+    <hyperlink ref="O25" r:id="rId106"/>
+    <hyperlink ref="O24" r:id="rId107"/>
+    <hyperlink ref="O23" r:id="rId108"/>
+    <hyperlink ref="O22" r:id="rId109"/>
+    <hyperlink ref="O21" r:id="rId110"/>
+    <hyperlink ref="O20" r:id="rId111"/>
+    <hyperlink ref="O19" r:id="rId112"/>
+    <hyperlink ref="O18" r:id="rId113"/>
+    <hyperlink ref="O17" r:id="rId114"/>
+    <hyperlink ref="O16" r:id="rId115"/>
+    <hyperlink ref="J6" r:id="rId116"/>
+    <hyperlink ref="J7:J34" r:id="rId117" display="http://publications.europa.eu/resource/authority/access-right/PUBLIC"/>
+    <hyperlink ref="J35" r:id="rId118"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId119"/>
@@ -3156,7 +3199,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -3171,12 +3214,12 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -3186,7 +3229,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
@@ -3206,7 +3249,7 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
@@ -3256,17 +3299,17 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
@@ -3286,35 +3329,35 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Working on updating metadata
</commit_message>
<xml_diff>
--- a/working-files-data/package_create.xlsx
+++ b/working-files-data/package_create.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="249">
   <si>
     <t>title</t>
   </si>
@@ -235,9 +235,6 @@
     <t>Transportløyver</t>
   </si>
   <si>
-    <t>Alle norske transportører som har løyver for både nasjonal og internasjonal transport av gods og/eller personer.</t>
-  </si>
-  <si>
     <t>Trafikkskoler</t>
   </si>
   <si>
@@ -382,9 +379,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>NLOD-1.0</t>
-  </si>
-  <si>
     <t>notspecified</t>
   </si>
   <si>
@@ -392,9 +386,6 @@
   </si>
   <si>
     <t>Beate Øien</t>
-  </si>
-  <si>
-    <t>trafikk, statistikk</t>
   </si>
   <si>
     <t>other-at</t>
@@ -682,9 +673,6 @@
     <t>obligatorisk i svv</t>
   </si>
   <si>
-    <t>hm</t>
-  </si>
-  <si>
     <t>obligatorisk i svv - bruke felles-epost?</t>
   </si>
   <si>
@@ -698,6 +686,87 @@
   </si>
   <si>
     <t>erstattes av</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/language/ENG</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>TODO flere!</t>
+  </si>
+  <si>
+    <t>Bytt ut!</t>
+  </si>
+  <si>
+    <t>NLOD</t>
+  </si>
+  <si>
+    <t>organisasjons_enhet</t>
+  </si>
+  <si>
+    <t>datex@vegvesen.no</t>
+  </si>
+  <si>
+    <t>Droppe?</t>
+  </si>
+  <si>
+    <t>firmapost@vegvesen.no</t>
+  </si>
+  <si>
+    <t>trafikk, trafikksikkerhet</t>
+  </si>
+  <si>
+    <t>trafikk, statistikk, ulykker</t>
+  </si>
+  <si>
+    <t>trafikkdata@vegvesen.no</t>
+  </si>
+  <si>
+    <t>trafikk, statistikk, ferje</t>
+  </si>
+  <si>
+    <t>vardata, vegmeldinger</t>
+  </si>
+  <si>
+    <t>www-admin@vegvesen.no</t>
+  </si>
+  <si>
+    <t>Transportørregister med alle norske transportører som har løyver for både nasjonal og internasjonal transport av gods og/eller personer.</t>
+  </si>
+  <si>
+    <t>Pål Rosland</t>
+  </si>
+  <si>
+    <t>paal.rosland@vegvesen.no</t>
+  </si>
+  <si>
+    <t>Se liste over kontaktpersoner på nettsida</t>
+  </si>
+  <si>
+    <t>http://www.vegvesen.no/fag/Fokusomrader/Miljo+og+omgivelser/Nasjonal+verneplan/nasjonal-verneplan</t>
+  </si>
+  <si>
+    <t>vegmuseum@vegvesen.no</t>
+  </si>
+  <si>
+    <t>ssb@ssb.no</t>
+  </si>
+  <si>
+    <t>Tilgang</t>
+  </si>
+  <si>
+    <t>Brukernavn/passord</t>
+  </si>
+  <si>
+    <t>Ekstra: Adgangsbegrensning</t>
+  </si>
+  <si>
+    <t>Ekstra: Kanskje bruke denne til grupper, evt. til "maintainer"</t>
+  </si>
+  <si>
+    <t>statistikk,trafikk</t>
   </si>
 </sst>
 </file>
@@ -1208,23 +1277,41 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="21" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1272,18 +1359,7 @@
     <cellStyle name="Uthevingsfarge6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Varseltekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -1571,1601 +1647,1763 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD35"/>
+  <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14 A1:XFD1"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:Y1"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.875" style="2" customWidth="1"/>
     <col min="4" max="4" width="56" style="2" customWidth="1"/>
-    <col min="5" max="9" width="12.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="42.125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="53.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.25" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="11" style="1"/>
+    <col min="5" max="6" width="12.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20" style="2" customWidth="1"/>
+    <col min="8" max="11" width="12.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="42.125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="53.75" style="2" customWidth="1"/>
+    <col min="16" max="16" width="20.25" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="5" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="6" customFormat="1" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="Y1" s="14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="9" spans="1:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
+    </row>
+    <row r="10" spans="1:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T19" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q20" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q21" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T21" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q24" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="U25" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q26" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T26" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q27" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="2:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q28" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T28" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="2:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T29" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q30" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q31" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T31" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="32" spans="2:27" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q32" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA32" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:32" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q33" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T33" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="2:32" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q34" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="2:32" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q35" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="2:32" s="4" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="E36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M3" t="s">
-        <v>166</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="G36" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q36" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="R36" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="51" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" t="s">
-        <v>163</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" t="s">
-        <v>168</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M8" t="s">
-        <v>169</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" t="s">
-        <v>170</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="M11" t="s">
-        <v>172</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M12" t="s">
-        <v>173</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M13" t="s">
-        <v>174</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="O23" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O26" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O27" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="O29" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O30" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="O31" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O32" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="2:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="2:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G34" s="4" t="s">
+      <c r="S36" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="T36" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O34" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="2:30" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="H35" s="9" t="s">
+      <c r="U36" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="V36" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="I35" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="L35" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="M35" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="N35" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="P35" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q35" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="R35" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="S35" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="T35" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="U35" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="AD35" s="12"/>
+      <c r="W36" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF36" s="12"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AI34">
-    <sortCondition ref="M2:M34"/>
+  <sortState ref="A4:AF35">
+    <sortCondition ref="B4:B35"/>
   </sortState>
-  <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="obligatorisk">
-      <formula>NOT(ISERROR(SEARCH("obligatorisk",A1)))</formula>
+  <conditionalFormatting sqref="A2:XFD2">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="obligatorisk">
+      <formula>NOT(ISERROR(SEARCH("obligatorisk",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N6" r:id="rId1"/>
-    <hyperlink ref="M14" r:id="rId2"/>
-    <hyperlink ref="M10" r:id="rId3"/>
-    <hyperlink ref="G3" r:id="rId4"/>
-    <hyperlink ref="G4" r:id="rId5"/>
-    <hyperlink ref="G5" r:id="rId6"/>
-    <hyperlink ref="G6" r:id="rId7"/>
-    <hyperlink ref="G7" r:id="rId8"/>
-    <hyperlink ref="G8" r:id="rId9"/>
-    <hyperlink ref="G9" r:id="rId10"/>
-    <hyperlink ref="G10" r:id="rId11"/>
-    <hyperlink ref="G11" r:id="rId12"/>
-    <hyperlink ref="G12" r:id="rId13"/>
-    <hyperlink ref="G13" r:id="rId14"/>
-    <hyperlink ref="G14" r:id="rId15"/>
-    <hyperlink ref="G35" r:id="rId16"/>
-    <hyperlink ref="G15" r:id="rId17"/>
-    <hyperlink ref="G16" r:id="rId18"/>
-    <hyperlink ref="G17" r:id="rId19"/>
-    <hyperlink ref="G18" r:id="rId20"/>
-    <hyperlink ref="G19" r:id="rId21"/>
-    <hyperlink ref="G20" r:id="rId22"/>
-    <hyperlink ref="G21" r:id="rId23"/>
-    <hyperlink ref="G22" r:id="rId24"/>
-    <hyperlink ref="G23" r:id="rId25"/>
-    <hyperlink ref="G24" r:id="rId26"/>
-    <hyperlink ref="G25" r:id="rId27"/>
-    <hyperlink ref="G26" r:id="rId28"/>
-    <hyperlink ref="G27" r:id="rId29"/>
-    <hyperlink ref="G28" r:id="rId30"/>
-    <hyperlink ref="G29" r:id="rId31"/>
-    <hyperlink ref="G30" r:id="rId32"/>
-    <hyperlink ref="G31" r:id="rId33"/>
-    <hyperlink ref="G32" r:id="rId34"/>
-    <hyperlink ref="G33" r:id="rId35"/>
-    <hyperlink ref="G34" r:id="rId36"/>
-    <hyperlink ref="R3" r:id="rId37"/>
-    <hyperlink ref="R4" r:id="rId38"/>
-    <hyperlink ref="R5" r:id="rId39"/>
-    <hyperlink ref="R7" r:id="rId40"/>
-    <hyperlink ref="S6" r:id="rId41"/>
-    <hyperlink ref="R8" r:id="rId42"/>
-    <hyperlink ref="R9" r:id="rId43"/>
-    <hyperlink ref="R10" r:id="rId44"/>
-    <hyperlink ref="R11" r:id="rId45"/>
-    <hyperlink ref="R12" r:id="rId46"/>
-    <hyperlink ref="R13" r:id="rId47"/>
-    <hyperlink ref="R14" r:id="rId48"/>
-    <hyperlink ref="R35" r:id="rId49"/>
-    <hyperlink ref="S35" r:id="rId50"/>
-    <hyperlink ref="F3" r:id="rId51"/>
-    <hyperlink ref="F4" r:id="rId52"/>
-    <hyperlink ref="F5" r:id="rId53"/>
-    <hyperlink ref="F6" r:id="rId54"/>
-    <hyperlink ref="F7" r:id="rId55"/>
-    <hyperlink ref="F8" r:id="rId56"/>
-    <hyperlink ref="F9" r:id="rId57"/>
-    <hyperlink ref="F10" r:id="rId58"/>
-    <hyperlink ref="F11" r:id="rId59"/>
-    <hyperlink ref="F34" r:id="rId60"/>
-    <hyperlink ref="F33" r:id="rId61"/>
-    <hyperlink ref="F32" r:id="rId62"/>
-    <hyperlink ref="F31" r:id="rId63"/>
-    <hyperlink ref="F30" r:id="rId64"/>
-    <hyperlink ref="F29" r:id="rId65"/>
-    <hyperlink ref="F17" r:id="rId66"/>
-    <hyperlink ref="F18" r:id="rId67"/>
-    <hyperlink ref="F19" r:id="rId68"/>
-    <hyperlink ref="F20" r:id="rId69"/>
-    <hyperlink ref="F21" r:id="rId70"/>
-    <hyperlink ref="F22" r:id="rId71"/>
-    <hyperlink ref="F23" r:id="rId72"/>
-    <hyperlink ref="F24" r:id="rId73"/>
-    <hyperlink ref="F25" r:id="rId74"/>
-    <hyperlink ref="F26" r:id="rId75"/>
-    <hyperlink ref="F27" r:id="rId76"/>
-    <hyperlink ref="F28" r:id="rId77"/>
-    <hyperlink ref="F12" r:id="rId78"/>
-    <hyperlink ref="F13" r:id="rId79"/>
-    <hyperlink ref="F14" r:id="rId80"/>
-    <hyperlink ref="F15" r:id="rId81"/>
-    <hyperlink ref="F16" r:id="rId82"/>
-    <hyperlink ref="O3" r:id="rId83"/>
-    <hyperlink ref="O4" r:id="rId84"/>
-    <hyperlink ref="O5" r:id="rId85"/>
-    <hyperlink ref="O6" r:id="rId86"/>
-    <hyperlink ref="O7" r:id="rId87"/>
-    <hyperlink ref="O8" r:id="rId88"/>
-    <hyperlink ref="O9" r:id="rId89"/>
-    <hyperlink ref="O10" r:id="rId90"/>
-    <hyperlink ref="O11" r:id="rId91"/>
-    <hyperlink ref="O12" r:id="rId92"/>
-    <hyperlink ref="O13" r:id="rId93"/>
-    <hyperlink ref="O14" r:id="rId94"/>
-    <hyperlink ref="O35" r:id="rId95"/>
-    <hyperlink ref="O15" r:id="rId96"/>
-    <hyperlink ref="O34" r:id="rId97"/>
-    <hyperlink ref="O33" r:id="rId98"/>
-    <hyperlink ref="O32" r:id="rId99"/>
-    <hyperlink ref="O31" r:id="rId100"/>
-    <hyperlink ref="O30" r:id="rId101"/>
-    <hyperlink ref="O29" r:id="rId102"/>
-    <hyperlink ref="O28" r:id="rId103"/>
-    <hyperlink ref="O27" r:id="rId104"/>
-    <hyperlink ref="O26" r:id="rId105"/>
-    <hyperlink ref="O25" r:id="rId106"/>
-    <hyperlink ref="O24" r:id="rId107"/>
-    <hyperlink ref="O23" r:id="rId108"/>
-    <hyperlink ref="O22" r:id="rId109"/>
-    <hyperlink ref="O21" r:id="rId110"/>
-    <hyperlink ref="O20" r:id="rId111"/>
-    <hyperlink ref="O19" r:id="rId112"/>
-    <hyperlink ref="O18" r:id="rId113"/>
-    <hyperlink ref="O17" r:id="rId114"/>
-    <hyperlink ref="O16" r:id="rId115"/>
-    <hyperlink ref="J6" r:id="rId116"/>
-    <hyperlink ref="J7:J34" r:id="rId117" display="http://publications.europa.eu/resource/authority/access-right/PUBLIC"/>
-    <hyperlink ref="J35" r:id="rId118"/>
+    <hyperlink ref="P15" r:id="rId1"/>
+    <hyperlink ref="O6" r:id="rId2"/>
+    <hyperlink ref="O28" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G5" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G15" r:id="rId7"/>
+    <hyperlink ref="G19" r:id="rId8"/>
+    <hyperlink ref="G21" r:id="rId9"/>
+    <hyperlink ref="G26" r:id="rId10"/>
+    <hyperlink ref="G28" r:id="rId11"/>
+    <hyperlink ref="G29" r:id="rId12"/>
+    <hyperlink ref="G31" r:id="rId13"/>
+    <hyperlink ref="G33" r:id="rId14"/>
+    <hyperlink ref="G6" r:id="rId15"/>
+    <hyperlink ref="G36" r:id="rId16"/>
+    <hyperlink ref="G25" r:id="rId17"/>
+    <hyperlink ref="G35" r:id="rId18"/>
+    <hyperlink ref="G8" r:id="rId19"/>
+    <hyperlink ref="G12" r:id="rId20"/>
+    <hyperlink ref="G9" r:id="rId21"/>
+    <hyperlink ref="G10" r:id="rId22"/>
+    <hyperlink ref="G11" r:id="rId23"/>
+    <hyperlink ref="G13" r:id="rId24"/>
+    <hyperlink ref="G14" r:id="rId25"/>
+    <hyperlink ref="G16" r:id="rId26"/>
+    <hyperlink ref="G17" r:id="rId27"/>
+    <hyperlink ref="G18" r:id="rId28"/>
+    <hyperlink ref="G20" r:id="rId29"/>
+    <hyperlink ref="G22" r:id="rId30"/>
+    <hyperlink ref="G23" r:id="rId31"/>
+    <hyperlink ref="G27" r:id="rId32"/>
+    <hyperlink ref="G24" r:id="rId33"/>
+    <hyperlink ref="G30" r:id="rId34"/>
+    <hyperlink ref="G34" r:id="rId35"/>
+    <hyperlink ref="G32" r:id="rId36"/>
+    <hyperlink ref="T4" r:id="rId37"/>
+    <hyperlink ref="T5" r:id="rId38"/>
+    <hyperlink ref="T7" r:id="rId39"/>
+    <hyperlink ref="T19" r:id="rId40"/>
+    <hyperlink ref="U15" r:id="rId41"/>
+    <hyperlink ref="T21" r:id="rId42"/>
+    <hyperlink ref="T26" r:id="rId43"/>
+    <hyperlink ref="T28" r:id="rId44"/>
+    <hyperlink ref="T29" r:id="rId45"/>
+    <hyperlink ref="T31" r:id="rId46"/>
+    <hyperlink ref="T33" r:id="rId47"/>
+    <hyperlink ref="T6" r:id="rId48"/>
+    <hyperlink ref="T36" r:id="rId49"/>
+    <hyperlink ref="U36" r:id="rId50"/>
+    <hyperlink ref="F4" r:id="rId51"/>
+    <hyperlink ref="F5" r:id="rId52"/>
+    <hyperlink ref="F7" r:id="rId53"/>
+    <hyperlink ref="F15" r:id="rId54"/>
+    <hyperlink ref="F19" r:id="rId55"/>
+    <hyperlink ref="F21" r:id="rId56"/>
+    <hyperlink ref="F26" r:id="rId57"/>
+    <hyperlink ref="F28" r:id="rId58"/>
+    <hyperlink ref="F29" r:id="rId59"/>
+    <hyperlink ref="F32" r:id="rId60"/>
+    <hyperlink ref="F34" r:id="rId61"/>
+    <hyperlink ref="F30" r:id="rId62"/>
+    <hyperlink ref="F24" r:id="rId63"/>
+    <hyperlink ref="F27" r:id="rId64"/>
+    <hyperlink ref="F23" r:id="rId65"/>
+    <hyperlink ref="F8" r:id="rId66"/>
+    <hyperlink ref="F12" r:id="rId67"/>
+    <hyperlink ref="F9" r:id="rId68"/>
+    <hyperlink ref="F10" r:id="rId69"/>
+    <hyperlink ref="F11" r:id="rId70"/>
+    <hyperlink ref="F13" r:id="rId71"/>
+    <hyperlink ref="F14" r:id="rId72"/>
+    <hyperlink ref="F16" r:id="rId73"/>
+    <hyperlink ref="F17" r:id="rId74"/>
+    <hyperlink ref="F18" r:id="rId75"/>
+    <hyperlink ref="F20" r:id="rId76"/>
+    <hyperlink ref="F22" r:id="rId77"/>
+    <hyperlink ref="F31" r:id="rId78"/>
+    <hyperlink ref="F33" r:id="rId79"/>
+    <hyperlink ref="F6" r:id="rId80"/>
+    <hyperlink ref="F25" r:id="rId81"/>
+    <hyperlink ref="F35" r:id="rId82"/>
+    <hyperlink ref="Q4" r:id="rId83"/>
+    <hyperlink ref="Q5" r:id="rId84"/>
+    <hyperlink ref="Q7" r:id="rId85"/>
+    <hyperlink ref="Q15" r:id="rId86"/>
+    <hyperlink ref="Q19" r:id="rId87"/>
+    <hyperlink ref="Q21" r:id="rId88"/>
+    <hyperlink ref="Q26" r:id="rId89"/>
+    <hyperlink ref="Q28" r:id="rId90"/>
+    <hyperlink ref="Q29" r:id="rId91"/>
+    <hyperlink ref="Q31" r:id="rId92"/>
+    <hyperlink ref="Q33" r:id="rId93"/>
+    <hyperlink ref="Q6" r:id="rId94"/>
+    <hyperlink ref="Q36" r:id="rId95"/>
+    <hyperlink ref="Q25" r:id="rId96"/>
+    <hyperlink ref="Q32" r:id="rId97"/>
+    <hyperlink ref="Q34" r:id="rId98"/>
+    <hyperlink ref="Q30" r:id="rId99"/>
+    <hyperlink ref="Q24" r:id="rId100"/>
+    <hyperlink ref="Q27" r:id="rId101"/>
+    <hyperlink ref="Q23" r:id="rId102"/>
+    <hyperlink ref="Q22" r:id="rId103"/>
+    <hyperlink ref="Q20" r:id="rId104"/>
+    <hyperlink ref="Q18" r:id="rId105"/>
+    <hyperlink ref="Q17" r:id="rId106"/>
+    <hyperlink ref="Q16" r:id="rId107"/>
+    <hyperlink ref="Q14" r:id="rId108"/>
+    <hyperlink ref="Q13" r:id="rId109"/>
+    <hyperlink ref="Q11" r:id="rId110"/>
+    <hyperlink ref="Q10" r:id="rId111"/>
+    <hyperlink ref="Q9" r:id="rId112"/>
+    <hyperlink ref="Q12" r:id="rId113"/>
+    <hyperlink ref="Q8" r:id="rId114"/>
+    <hyperlink ref="Q35" r:id="rId115"/>
+    <hyperlink ref="L15" r:id="rId116"/>
+    <hyperlink ref="L8:L35" r:id="rId117" display="http://publications.europa.eu/resource/authority/access-right/PUBLIC"/>
+    <hyperlink ref="L36" r:id="rId118"/>
+    <hyperlink ref="I9" r:id="rId119"/>
+    <hyperlink ref="I12" r:id="rId120"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId119"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId121"/>
 </worksheet>
 </file>
 
@@ -3184,7 +3422,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -3199,27 +3437,27 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -3229,27 +3467,27 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
@@ -3279,7 +3517,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
@@ -3299,17 +3537,17 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
@@ -3329,12 +3567,12 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
@@ -3342,22 +3580,22 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>